<commit_message>
Group Modified by Location
</commit_message>
<xml_diff>
--- a/Groups.xlsx
+++ b/Groups.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Groups" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="NewGroups" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Groups" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t xml:space="preserve">Group No.</t>
   </si>
@@ -40,118 +41,118 @@
     <t xml:space="preserve">BA-01</t>
   </si>
   <si>
+    <t xml:space="preserve">Hindu Bojanki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raghunath Gudimetta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pancharatna Magdum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaurav Shrisunder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Praveen Gupta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ritul De</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swarupa Veturlekar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amol Sutar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pranjal Negi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashish Kavathekar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sk Arman  Hossain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anamika Biswas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Md Azhar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binoy Kumar Mondal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subhadip Nayek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deepak Prasad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adarsh Rao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vijay Ingle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akil Bandgar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinaya Mahale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amardeep Lokare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhisek Mahato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohan Sen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arumita Mitra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sabyasachi Sanki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swarnali Ghosh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suman Rana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pritish Tare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devesh Maithani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nilam Mhambare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prasanna Argade</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shridhar Banne</t>
   </si>
   <si>
     <t xml:space="preserve">Abhijeet Sanjay Neje</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ashish Kavathekar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suman Rana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindu Bojanki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Praveen Gupta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ritul De</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swarupa Veturlekar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amol Sutar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaurav Shrisunder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vijay Ingle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akil Bandgar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anamika Biswas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amardeep Lokare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Md Azhar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pranjal Negi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deepak Prasad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adarsh Rao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Binoy Kumar Mondal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subhadip Nayek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vinaya Mahale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sk Arman  Hossain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abhisek Mahato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohan Sen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pancharatna Magdum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sabyasachi Sanki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swarnali Ghosh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pritish Tare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA-06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arumita Mitra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devesh Maithani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nilam Mhambare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prasanna Argade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raghunath Gudimetta</t>
   </si>
 </sst>
 </file>
@@ -376,10 +377,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:AMJ43"/>
+  <dimension ref="B2:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -426,7 +427,7 @@
     </row>
     <row r="5" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="8"/>
@@ -448,17 +449,10 @@
       <c r="AMI6" s="10"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="8"/>
+    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="AMG7" s="10"/>
-      <c r="AMH7" s="10"/>
-      <c r="AMI7" s="10"/>
-      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="6" t="s">
@@ -466,21 +460,24 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2" t="n">
-        <v>2</v>
-      </c>
       <c r="C11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -512,15 +509,15 @@
       <c r="C18" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -540,9 +537,9 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="6"/>
@@ -552,38 +549,38 @@
         <v>4</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,54 +591,57 @@
         <v>5</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="2" t="n">
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>4</v>
@@ -649,16 +649,22 @@
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="6" t="s">
+      <c r="D43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -671,4 +677,300 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:AMJ43"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="46.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="36.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="7" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="AMH4" s="10"/>
+      <c r="AMI4" s="10"/>
+      <c r="AMJ4" s="10"/>
+    </row>
+    <row r="5" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="8"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="AMH5" s="10"/>
+      <c r="AMI5" s="10"/>
+      <c r="AMJ5" s="10"/>
+    </row>
+    <row r="6" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="8"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="AMH6" s="10"/>
+      <c r="AMI6" s="10"/>
+      <c r="AMJ6" s="10"/>
+    </row>
+    <row r="7" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="8"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="AMH7" s="10"/>
+      <c r="AMI7" s="10"/>
+      <c r="AMJ7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="17.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0"/>
+      <c r="C30" s="0"/>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0"/>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>